<commit_message>
update func display ep 🎬
</commit_message>
<xml_diff>
--- a/public/tmp/pivotclaim.xlsx
+++ b/public/tmp/pivotclaim.xlsx
@@ -836,13 +836,13 @@
         <v>20</v>
       </c>
       <c r="B12" s="2">
-        <v>597851.17</v>
+        <v>602271.17</v>
       </c>
       <c r="C12" s="2">
-        <v>562326.45</v>
+        <v>562465.85</v>
       </c>
       <c r="D12" s="2">
-        <v>1160177.62</v>
+        <v>1164737.02</v>
       </c>
       <c r="E12" s="2">
         <v>76</v>

</xml_diff>